<commit_message>
added the excel sheet for prostate cancer drugs analogs
</commit_message>
<xml_diff>
--- a/Prostate Cancer Drugs Analogs.xlsx
+++ b/Prostate Cancer Drugs Analogs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hp\Documents\Biomedical Engineering\Noguchi Internship\Drug Repurposing\drug-repurposing\drug_repurposing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51F80EF5-9AF6-42A6-A242-E895F835D9AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82D3A32C-347D-42AB-B943-C5FBA082EAC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="768" yWindow="768" windowWidth="9720" windowHeight="12192" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,12 +25,114 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="36">
   <si>
     <t>PRECURSOR DRUG COMPOUND</t>
   </si>
   <si>
-    <t>ANALOGOUS DRUG COMPOUNDS</t>
+    <t>DEGARELIX</t>
+  </si>
+  <si>
+    <t>ACYLINE</t>
+  </si>
+  <si>
+    <t>SATEREOTIDE TETRAXETAN</t>
+  </si>
+  <si>
+    <t>CETRORELIX</t>
+  </si>
+  <si>
+    <t>GANIRELIX</t>
+  </si>
+  <si>
+    <t>ANALOGOUS DRUG COMPOUND</t>
+  </si>
+  <si>
+    <t>DESLORELIN</t>
+  </si>
+  <si>
+    <t>NAFARELIN</t>
+  </si>
+  <si>
+    <t>GONADORELIN</t>
+  </si>
+  <si>
+    <t>AFAMELANOTIDE</t>
+  </si>
+  <si>
+    <t>ALSACTIDE</t>
+  </si>
+  <si>
+    <t>CZEN 202</t>
+  </si>
+  <si>
+    <t>MODIMELANOTIDE</t>
+  </si>
+  <si>
+    <t>TASPOGLUTIDE</t>
+  </si>
+  <si>
+    <t>TETRACOSACTIDE</t>
+  </si>
+  <si>
+    <t>BREMELANOTIDE</t>
+  </si>
+  <si>
+    <t>COTATDUTIDE</t>
+  </si>
+  <si>
+    <t>TRIDECTIDE</t>
+  </si>
+  <si>
+    <t>AMY-101</t>
+  </si>
+  <si>
+    <t>TRY-120027</t>
+  </si>
+  <si>
+    <t>ANGIOTENSINAMIDE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SEMAGLUTIDE </t>
+  </si>
+  <si>
+    <t>ALBUVIRTIDE</t>
+  </si>
+  <si>
+    <t>ANGIOTENSIN 1-7</t>
+  </si>
+  <si>
+    <t>LIXISENATIDE</t>
+  </si>
+  <si>
+    <t>SETMELANOTIDE</t>
+  </si>
+  <si>
+    <t>SARALASIN</t>
+  </si>
+  <si>
+    <t>PRAMLINTIDE</t>
+  </si>
+  <si>
+    <t>MUREPAVADIN</t>
+  </si>
+  <si>
+    <t>ELIGARD (LEUPROLIDE ACETATE)</t>
+  </si>
+  <si>
+    <t>(R)-3-BROMO-2-HYDROXY-2-METHYL-N-[4-NITRO-3-(TRIFLUOROMETHYL)PHENYL]PROPANAMIDE AND CANCER</t>
+  </si>
+  <si>
+    <t>FLUTAMIDE</t>
+  </si>
+  <si>
+    <t>ANGIOTENSIN II</t>
+  </si>
+  <si>
+    <t>ACLERASTIDE</t>
+  </si>
+  <si>
+    <t>GOSERELIN ACETATE</t>
   </si>
 </sst>
 </file>
@@ -359,16 +461,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.77734375" customWidth="1"/>
-    <col min="2" max="2" width="31.5546875" customWidth="1"/>
+    <col min="1" max="1" width="13" customWidth="1"/>
+    <col min="2" max="2" width="20.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" s="1" customFormat="1" ht="39.6" customHeight="1" x14ac:dyDescent="0.3">
@@ -376,7 +478,247 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>30</v>
+      </c>
+      <c r="B27" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>35</v>
+      </c>
+      <c r="B31" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>